<commit_message>
GIZ-255: decimal.js for lw calculations
</commit_message>
<xml_diff>
--- a/test/import-excels/giz-calc-20w-mixed-perc-mixed-gap.xlsx
+++ b/test/import-excels/giz-calc-20w-mixed-perc-mixed-gap.xlsx
@@ -415,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -544,37 +544,6 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="12"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="12"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="medium">
-        <color indexed="12"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
       <right style="medium">
         <color indexed="12"/>
       </right>
@@ -652,7 +621,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -722,46 +691,31 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2191,7 +2145,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:BD10"/>
+  <dimension ref="A1:BD6"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2800,238 +2754,6 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
-      <c r="AA7" s="4"/>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="24"/>
-      <c r="AE7" s="4"/>
-      <c r="AF7" s="24"/>
-      <c r="AG7" s="4"/>
-      <c r="AH7" s="24"/>
-      <c r="AI7" s="4"/>
-      <c r="AJ7" s="24"/>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="24"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="24"/>
-      <c r="AO7" s="24"/>
-      <c r="AP7" s="4"/>
-      <c r="AQ7" s="24"/>
-      <c r="AR7" s="24"/>
-      <c r="AS7" s="24"/>
-      <c r="AT7" s="24"/>
-      <c r="AU7" s="4"/>
-      <c r="AV7" s="24"/>
-      <c r="AW7" s="24"/>
-      <c r="AX7" s="24"/>
-      <c r="AY7" s="24"/>
-      <c r="AZ7" s="4"/>
-      <c r="BA7" s="24"/>
-      <c r="BB7" s="24"/>
-      <c r="BC7" s="4"/>
-      <c r="BD7" s="25"/>
-    </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-      <c r="AA8" s="8"/>
-      <c r="AB8" s="8"/>
-      <c r="AC8" s="8"/>
-      <c r="AD8" s="8"/>
-      <c r="AE8" s="8"/>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AH8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
-      <c r="AK8" s="8"/>
-      <c r="AL8" s="8"/>
-      <c r="AM8" s="8"/>
-      <c r="AN8" s="8"/>
-      <c r="AO8" s="8"/>
-      <c r="AP8" s="8"/>
-      <c r="AQ8" s="8"/>
-      <c r="AR8" s="8"/>
-      <c r="AS8" s="8"/>
-      <c r="AT8" s="8"/>
-      <c r="AU8" s="8"/>
-      <c r="AV8" s="8"/>
-      <c r="AW8" s="8"/>
-      <c r="AX8" s="8"/>
-      <c r="AY8" s="8"/>
-      <c r="AZ8" s="8"/>
-      <c r="BA8" s="8"/>
-      <c r="BB8" s="8"/>
-      <c r="BC8" s="8"/>
-      <c r="BD8" s="9"/>
-    </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
-      <c r="AA9" s="8"/>
-      <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="8"/>
-      <c r="AE9" s="8"/>
-      <c r="AF9" s="8"/>
-      <c r="AG9" s="8"/>
-      <c r="AH9" s="8"/>
-      <c r="AI9" s="8"/>
-      <c r="AJ9" s="8"/>
-      <c r="AK9" s="8"/>
-      <c r="AL9" s="8"/>
-      <c r="AM9" s="8"/>
-      <c r="AN9" s="8"/>
-      <c r="AO9" s="8"/>
-      <c r="AP9" s="8"/>
-      <c r="AQ9" s="8"/>
-      <c r="AR9" s="8"/>
-      <c r="AS9" s="8"/>
-      <c r="AT9" s="8"/>
-      <c r="AU9" s="8"/>
-      <c r="AV9" s="8"/>
-      <c r="AW9" s="8"/>
-      <c r="AX9" s="8"/>
-      <c r="AY9" s="8"/>
-      <c r="AZ9" s="8"/>
-      <c r="BA9" s="8"/>
-      <c r="BB9" s="8"/>
-      <c r="BC9" s="8"/>
-      <c r="BD9" s="9"/>
-    </row>
-    <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="13"/>
-      <c r="AI10" s="13"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="13"/>
-      <c r="AL10" s="13"/>
-      <c r="AM10" s="13"/>
-      <c r="AN10" s="13"/>
-      <c r="AO10" s="13"/>
-      <c r="AP10" s="13"/>
-      <c r="AQ10" s="13"/>
-      <c r="AR10" s="13"/>
-      <c r="AS10" s="13"/>
-      <c r="AT10" s="13"/>
-      <c r="AU10" s="13"/>
-      <c r="AV10" s="13"/>
-      <c r="AW10" s="13"/>
-      <c r="AX10" s="13"/>
-      <c r="AY10" s="13"/>
-      <c r="AZ10" s="13"/>
-      <c r="BA10" s="13"/>
-      <c r="BB10" s="13"/>
-      <c r="BC10" s="13"/>
-      <c r="BD10" s="14"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -3052,19 +2774,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="20" style="28" customWidth="1"/>
-    <col min="7" max="16384" width="8.85156" style="28" customWidth="1"/>
+    <col min="1" max="6" width="20" style="23" customWidth="1"/>
+    <col min="7" max="16384" width="8.85156" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
-      <c r="A1" t="s" s="29">
+      <c r="A1" t="s" s="24">
         <v>109</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="19">
@@ -3082,25 +2804,25 @@
       <c r="E2" t="s" s="19">
         <v>114</v>
       </c>
-      <c r="F2" t="s" s="31">
+      <c r="F2" t="s" s="26">
         <v>115</v>
       </c>
     </row>
     <row r="3" ht="10" customHeight="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="18"/>
@@ -3108,7 +2830,7 @@
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
-      <c r="F5" s="36"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="18"/>
@@ -3116,7 +2838,7 @@
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
-      <c r="F6" s="36"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="18"/>
@@ -3124,7 +2846,7 @@
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="36"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="18"/>
@@ -3132,7 +2854,7 @@
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="36"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="18"/>
@@ -3140,7 +2862,7 @@
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="36"/>
+      <c r="F9" s="31"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="18"/>
@@ -3148,7 +2870,7 @@
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="36"/>
+      <c r="F10" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>